<commit_message>
Atualização do arquivo aula 10 com novos fluxos
</commit_message>
<xml_diff>
--- a/aula10_ desenvolvidoTestCase_UseCase.xlsx
+++ b/aula10_ desenvolvidoTestCase_UseCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Automacao\TestesExploratorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35DEAA3-91E4-43F6-BD0B-CCC7744B5AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D8535-7370-4953-A0EA-73B776C0183A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8B4C74CC-E034-4090-999E-01782DB39DF4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Fluxo</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Fluxos Aluno</t>
   </si>
   <si>
-    <t>[FE6][FE7]</t>
-  </si>
-  <si>
     <t>[FE5][FE8]</t>
   </si>
   <si>
@@ -188,6 +185,39 @@
   </si>
   <si>
     <t>Disparar e-mail para o usuário com dados do pedido</t>
+  </si>
+  <si>
+    <t>[FA6]</t>
+  </si>
+  <si>
+    <t>Alterar depois Remover a quantidade do Item e adicionar para ver se a soma está OK</t>
+  </si>
+  <si>
+    <t>[FE11]</t>
+  </si>
+  <si>
+    <t>CEP informado {Alphanumérico, Caracteres Especiais, Com Espaço e etc}</t>
+  </si>
+  <si>
+    <t>[FA7]</t>
+  </si>
+  <si>
+    <t>Incluir novos itens (3 itens) depois Remover a quantidade e adicionar para ver se a soma está OK</t>
+  </si>
+  <si>
+    <t>[SIS_ERROR]</t>
+  </si>
+  <si>
+    <t>Não preencher o(s) campo(s) obrigatórios</t>
+  </si>
+  <si>
+    <t>[FE4][FA2][FA6][FA7]</t>
+  </si>
+  <si>
+    <t>[FE4][FE6][FE7][FE11]</t>
+  </si>
+  <si>
+    <t>Não apresenta a interface do "Pedido" quando acessado. Evento de inoperabilidade que pode ser testado simulando falta do DB, Back ou alguma aplicação para o funcionamento deste Sistema.</t>
   </si>
 </sst>
 </file>
@@ -281,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,6 +324,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,8 +453,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8539079" y="296445"/>
-          <a:ext cx="1121276" cy="4623134"/>
+          <a:off x="8980237" y="296445"/>
+          <a:ext cx="1121276" cy="4990766"/>
           <a:chOff x="9010650" y="234950"/>
           <a:chExt cx="1123950" cy="4552950"/>
         </a:xfrm>
@@ -1553,22 +1601,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F01B-6553-4E8C-A755-ACE048DCE152}">
-  <dimension ref="B1:E29"/>
+  <dimension ref="B1:E34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
     <col min="3" max="3" width="60.1796875" customWidth="1"/>
     <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="17" x14ac:dyDescent="0.4">
       <c r="B2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1576,7 +1625,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1596,7 +1645,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
@@ -1610,7 +1659,7 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
@@ -1621,7 +1670,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
@@ -1635,7 +1684,7 @@
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
@@ -1649,7 +1698,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
@@ -1660,7 +1709,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
@@ -1703,92 +1752,124 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>3</v>
+    <row r="18" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="4" t="s">
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="6" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="7" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="11" t="s">
         <v>50</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1877,15 +1958,15 @@
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.35">
@@ -1901,7 +1982,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.35">
@@ -1914,10 +1995,10 @@
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>